<commit_message>
added interface to ProjectObjects.xlsx
</commit_message>
<xml_diff>
--- a/ProjectObjects.xlsx
+++ b/ProjectObjects.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Class" sheetId="1" r:id="rId1"/>
+    <sheet name="Interface" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Program</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>Hero</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Damage</t>
   </si>
 </sst>
 </file>
@@ -110,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,11 +140,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,6 +185,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -739,6 +796,170 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E95425-0F80-4001-B622-7A5FBF08EDC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7429500" y="1857375"/>
+          <a:ext cx="7429501" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>704851</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70F30CC8-F379-4B02-8C16-CD650953AAF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3714750" y="2238375"/>
+          <a:ext cx="2933701" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1476375</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5248FF7D-ED5B-489A-AFC8-294CFFAD7699}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4448175" y="2971800"/>
+          <a:ext cx="1495425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1049,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1109,4 +1330,113 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="22.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="5" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="C12" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added keyboard to ProjectObjects.xlsx
</commit_message>
<xml_diff>
--- a/ProjectObjects.xlsx
+++ b/ProjectObjects.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Class" sheetId="1" r:id="rId1"/>
     <sheet name="Interface" sheetId="2" r:id="rId2"/>
+    <sheet name="Keyboard Entries" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Program</t>
   </si>
@@ -70,6 +71,48 @@
   </si>
   <si>
     <t>Damage</t>
+  </si>
+  <si>
+    <t>Spacebar</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 1</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 2</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 3</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 4</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 5</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 6</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 7</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 8</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 9</t>
+  </si>
+  <si>
+    <t>Upgrade Hero 10</t>
+  </si>
+  <si>
+    <t>Level UP</t>
   </si>
 </sst>
 </file>
@@ -187,6 +230,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,18 +252,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1336,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1346,86 +1389,81 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="A3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="5" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="A6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="E5:E6"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A6"/>
@@ -1434,9 +1472,103 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="17.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>